<commit_message>
Student Routing and more...
- Move the student blade files to their own folders
- Edited the routing
- Added Create Quiz for the teacher.
- All of the migration files are working with foreign key.
- Various Design Choices.
- Model Changes.
- Added sidenavbar for students
- Basta madaming nagbago, nakalagay naman eh
</commit_message>
<xml_diff>
--- a/public/files/Template.xlsx
+++ b/public/files/Template.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="StudentSheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>BSIT</t>
   </si>
   <si>
-    <t>4A</t>
-  </si>
-  <si>
     <t>2017-2018</t>
   </si>
   <si>
@@ -44,22 +41,25 @@
     <t>Cruz, Aimee Lou D.</t>
   </si>
   <si>
-    <t>course</t>
-  </si>
-  <si>
-    <t>section</t>
-  </si>
-  <si>
-    <t>year</t>
-  </si>
-  <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>3A</t>
+  </si>
+  <si>
+    <t>class_course</t>
+  </si>
+  <si>
+    <t>class_section</t>
+  </si>
+  <si>
+    <t>class_school_year</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -413,73 +413,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" customWidth="1"/>
-    <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Another MASSIVE UPDATE Hereee...
- Edited some Controllers
- Added AOS Animation
- Added and edited some colors
- Seperated the designer css and js file
- Some styles
- Finally added a working Simulator using Web SQL
- A working but buggy SQL Designer
- Change Password works
- Part of the Quiz Module
- Added Audit Trail
- Fixed Downloads
- Design Choices
- Minor Fixes...
</commit_message>
<xml_diff>
--- a/public/files/Template.xlsx
+++ b/public/files/Template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
-  <si>
-    <t>name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>class_course</t>
   </si>
@@ -44,143 +41,122 @@
     <t>*** NOTHING FOLLOWS***</t>
   </si>
   <si>
-    <r>
-      <t>BS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1" tint="0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>**</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1" tint="0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1" tint="0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>**</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-20</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1" tint="0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>**</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1" tint="0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>juandelacruz</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1" tint="0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>sample</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.com</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Dela Cruz, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1" tint="0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Juan</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> D.</t>
-    </r>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>middle_name</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>Nylle Brian</t>
+  </si>
+  <si>
+    <t>Rand1</t>
+  </si>
+  <si>
+    <t>Bague</t>
+  </si>
+  <si>
+    <t>James Darrell</t>
+  </si>
+  <si>
+    <t>Rand2</t>
+  </si>
+  <si>
+    <t>De Vera</t>
+  </si>
+  <si>
+    <t>nyllebrian@gmail.com</t>
+  </si>
+  <si>
+    <t>Khim</t>
+  </si>
+  <si>
+    <t>Rand3</t>
+  </si>
+  <si>
+    <t>Elbo</t>
+  </si>
+  <si>
+    <t>jamesdevera@gmail.com</t>
+  </si>
+  <si>
+    <t>khimelbo@gmail.com</t>
+  </si>
+  <si>
+    <t>Donald Patrick</t>
+  </si>
+  <si>
+    <t>Costa</t>
+  </si>
+  <si>
+    <t>George</t>
+  </si>
+  <si>
+    <t>donpatrick15@gmail.com</t>
+  </si>
+  <si>
+    <t>BSIT</t>
+  </si>
+  <si>
+    <t>3A</t>
+  </si>
+  <si>
+    <t>2017-2018</t>
+  </si>
+  <si>
+    <t>Jazelene Mae</t>
+  </si>
+  <si>
+    <t>Mercado</t>
+  </si>
+  <si>
+    <t>jazelenemae@gmail.com</t>
+  </si>
+  <si>
+    <t>Jeremiah</t>
+  </si>
+  <si>
+    <t>Rand4</t>
+  </si>
+  <si>
+    <t>Nicor</t>
+  </si>
+  <si>
+    <t>jmnicor@gmail.com</t>
+  </si>
+  <si>
+    <t>Gabriel</t>
+  </si>
+  <si>
+    <t>Rand5</t>
+  </si>
+  <si>
+    <t>Tabernilla</t>
+  </si>
+  <si>
+    <t>gabtab@gmail.com</t>
+  </si>
+  <si>
+    <t>Marlon Paolo</t>
+  </si>
+  <si>
+    <t>Rand6</t>
+  </si>
+  <si>
+    <t>Villamor</t>
+  </si>
+  <si>
+    <t>paolovillamor@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,13 +168,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1" tint="0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -224,10 +193,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -545,163 +517,287 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="E3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>